<commit_message>
Baseline, TestData, Login and HomePage Java
</commit_message>
<xml_diff>
--- a/src/main/java/testdata/Baseline File.xlsx
+++ b/src/main/java/testdata/Baseline File.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="30" windowWidth="20115" windowHeight="7755" firstSheet="4" activeTab="7"/>
+    <workbookView xWindow="240" yWindow="30" windowWidth="20115" windowHeight="7755"/>
   </bookViews>
   <sheets>
     <sheet name="HomePage" sheetId="4" r:id="rId1"/>
@@ -228,9 +228,6 @@
     <t>03192021 Company: 564!1Automation Subcontractor 1-DO NOT TOUCH: Missing!Allstate Striping &amp; Sealing Co: Missing!Bala Con T1 Entity#2: BALAT1-002!CentiMark Corporation: Missing!Comapany 2: Missing!D.E. Alston Enterprises LLC: Missing!Estime Enterprises, Inc: Missing!G&amp;M Services LLC: Missing!Hauling Unlimited, LLC: Missing!IN-1884 Subcontractor Tier 1: 1884!Jay &amp; Los Transport, LLC: Missing!Kara Test: C#3455555!Late Starter Sub: Missing!May Branch Test: Missing!Midwest Mole, Inc.: Missing!New Q3 Automation Subcontractor 10062021: 12347878!New Subcontractor: Missing!Oklahoma Sub: Missing!Pipefitters Inc: Missing!Q3 Tier 2 Subcontractor: Missing!RE Lee Electric Co, Inc. : Missing!S1New: Missing!Tawakal Transportation LLC: Missing!Test Tier 2: Missing!Union Sub: Missing!Vision Technologies, Inc.: Missing!White Car Sub: Missing!XYZ Company : Missing!YM Tier 2 Sub: Missing!Z-Best Wallcoverings, Inc.: Missing!</t>
   </si>
   <si>
-    <t>Basic Project!Copy Subs 2 Test!Copy Subs Project - Orchid!Mortenson Washington!No Entity Project!No Subs Project!P3 Test Project!Prev. Wage Project - All Features-new!RPAI Test Project 1!RPAI Test Project 2!Spring Copy Project!Wayne County Test Project</t>
-  </si>
-  <si>
     <t>PayrollSchedule</t>
   </si>
   <si>
@@ -277,6 +274,9 @@
   </si>
   <si>
     <t>Select...!Full Time Worker!Part Time Worker!Contract Worker!Temp Worker</t>
+  </si>
+  <si>
+    <t>Basic Project!Copy Subs 2 Test!Copy Subs Project - Orchid!Mortenson Washington!No Entity Project!No Subs Project!P3 Test Project!Prev. Wage Project - All Features-new!Clone of Prev. Wage Project - All Features-new!No Entity No Region Project!Spring Copy Project!Wayne County Test Project</t>
   </si>
 </sst>
 </file>
@@ -647,7 +647,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -660,7 +660,7 @@
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>49</v>
+        <v>65</v>
       </c>
     </row>
   </sheetData>
@@ -933,10 +933,10 @@
         <v>0</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>47</v>
@@ -968,13 +968,13 @@
         <v>2</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D2" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="E2" s="8" t="s">
         <v>53</v>
-      </c>
-      <c r="E2" s="8" t="s">
-        <v>54</v>
       </c>
       <c r="F2" s="4" t="s">
         <v>1</v>
@@ -1058,10 +1058,10 @@
         <v>26</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="G1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="2" spans="1:7" ht="409.5" x14ac:dyDescent="0.25">
@@ -1081,10 +1081,10 @@
         <v>30</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
   </sheetData>
@@ -1096,7 +1096,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="K2" sqref="K2"/>
     </sheetView>
   </sheetViews>
@@ -1122,24 +1122,24 @@
         <v>31</v>
       </c>
       <c r="F1" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>58</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>59</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="B2" s="3" t="s">
         <v>60</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>61</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>27</v>
@@ -1151,16 +1151,16 @@
         <v>32</v>
       </c>
       <c r="F2" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="H2" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="G2" s="1" t="s">
+      <c r="I2" s="1" t="s">
         <v>64</v>
-      </c>
-      <c r="H2" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="I2" s="1" t="s">
-        <v>65</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Employee Management,Baseline, UI Image
</commit_message>
<xml_diff>
--- a/src/main/java/testdata/Baseline File.xlsx
+++ b/src/main/java/testdata/Baseline File.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="81">
   <si>
     <t>Gender</t>
   </si>
@@ -304,6 +304,24 @@
   </si>
   <si>
     <t>ProjectReportingDateQuarterly</t>
+  </si>
+  <si>
+    <t>Attention</t>
+  </si>
+  <si>
+    <t>Show All!Needs a Wage Rate!Out of Compliance</t>
+  </si>
+  <si>
+    <t>Validated</t>
+  </si>
+  <si>
+    <t>Assigned to Project</t>
+  </si>
+  <si>
+    <t>Show All!Validated!Not Validated</t>
+  </si>
+  <si>
+    <t>Show All!Assigned!Not Assigned</t>
   </si>
 </sst>
 </file>
@@ -1171,72 +1189,90 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I2"/>
+  <dimension ref="A1:L2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K2" sqref="K2"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="9" width="9.140625" style="1"/>
+    <col min="1" max="12" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="409.5" x14ac:dyDescent="0.25">
-      <c r="A2" s="4" t="s">
+    <row r="2" spans="1:12" ht="409.5" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="D2" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="E2" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="F2" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="G2" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="H2" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="I2" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="G2" s="1" t="s">
+      <c r="J2" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="H2" s="1" t="s">
+      <c r="K2" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="I2" s="1" t="s">
+      <c r="L2" s="1" t="s">
         <v>63</v>
       </c>
     </row>

</xml_diff>